<commit_message>
la til en ny fil
</commit_message>
<xml_diff>
--- a/Årsplan IT2.xlsx
+++ b/Årsplan IT2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iktagder-my.sharepoint.com/personal/fredrik_pettersen_mandal_vgs_no/Documents/2023 - 2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iktagder-my.sharepoint.com/personal/fredrik_pettersen_mandal_vgs_no/Documents/2023 - 2024/IT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E593647-C825-4342-B68D-65F0866BA014}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="33">
   <si>
     <t>Arbeidsplan Naturfag 1IDA</t>
   </si>
@@ -112,6 +112,27 @@
   </si>
   <si>
     <t>1.skoledag</t>
+  </si>
+  <si>
+    <t>Vurdering</t>
+  </si>
+  <si>
+    <t>Prøve</t>
+  </si>
+  <si>
+    <t>Fagdag</t>
+  </si>
+  <si>
+    <t>Skrivedag, norsk</t>
+  </si>
+  <si>
+    <t>OD-dag</t>
+  </si>
+  <si>
+    <t>Volleyballturnering</t>
+  </si>
+  <si>
+    <t>Fagdag Blokk 4</t>
   </si>
 </sst>
 </file>
@@ -121,7 +142,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ mmm\."/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -184,7 +205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +248,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -479,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -563,9 +596,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -608,9 +638,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,9 +657,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,6 +722,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,18 +1073,18 @@
   <dimension ref="A1:S1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.21875" style="25" customWidth="1"/>
     <col min="2" max="3" width="9.5546875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" style="33" customWidth="1"/>
     <col min="8" max="8" width="26.77734375" style="25" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.77734375" style="25" bestFit="1" customWidth="1"/>
@@ -1039,31 +1096,31 @@
     <col min="17" max="18" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="62"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="59"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1078,7 +1135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1088,23 +1145,23 @@
       <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="9">
         <v>33</v>
       </c>
@@ -1114,18 +1171,18 @@
       <c r="C5" s="12">
         <v>45158</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="27"/>
+      <c r="H5" s="73"/>
       <c r="K5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="9">
         <v>34</v>
       </c>
@@ -1141,17 +1198,17 @@
       <c r="E6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="13"/>
       <c r="K6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="9">
         <v>35</v>
       </c>
@@ -1167,17 +1224,17 @@
       <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="13"/>
       <c r="K7" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="9">
         <v>36</v>
       </c>
@@ -1190,19 +1247,19 @@
       <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="27"/>
+      <c r="E8" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="72"/>
+      <c r="G8" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="73"/>
       <c r="K8" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="9">
         <v>37</v>
       </c>
@@ -1218,16 +1275,16 @@
       <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="73"/>
       <c r="K9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1">
       <c r="A10" s="9">
         <v>38</v>
       </c>
@@ -1243,18 +1300,18 @@
       <c r="E10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="73"/>
       <c r="I10" s="9"/>
       <c r="J10" s="25"/>
       <c r="K10" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="9">
         <v>39</v>
       </c>
@@ -1270,16 +1327,16 @@
       <c r="E11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="73"/>
       <c r="K11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="9">
         <v>40</v>
       </c>
@@ -1289,18 +1346,18 @@
       <c r="C12" s="14">
         <v>45207</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
       <c r="K12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="13">
         <v>41</v>
       </c>
@@ -1316,16 +1373,17 @@
       <c r="E13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="H13" s="74"/>
       <c r="I13" s="13"/>
       <c r="K13" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="13">
         <v>42</v>
       </c>
@@ -1341,18 +1399,18 @@
       <c r="E14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="46" t="s">
+      <c r="F14" s="72"/>
+      <c r="G14" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="13">
         <v>43</v>
       </c>
@@ -1365,20 +1423,20 @@
       <c r="D15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="13"/>
+      <c r="E15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="72"/>
       <c r="G15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="73"/>
       <c r="I15" s="13"/>
       <c r="K15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="13">
         <v>44</v>
       </c>
@@ -1394,16 +1452,16 @@
       <c r="E16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="27"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="73"/>
       <c r="K16" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="13">
         <v>45</v>
       </c>
@@ -1419,16 +1477,16 @@
       <c r="E17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="13"/>
+      <c r="F17" s="72"/>
       <c r="G17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="27"/>
+      <c r="H17" s="73"/>
       <c r="K17" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="13">
         <v>46</v>
       </c>
@@ -1444,16 +1502,16 @@
       <c r="E18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="72"/>
       <c r="G18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="73"/>
       <c r="K18" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="13">
         <v>47</v>
       </c>
@@ -1466,19 +1524,19 @@
       <c r="D19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="13"/>
+      <c r="E19" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="72"/>
       <c r="G19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="27"/>
+      <c r="H19" s="73"/>
       <c r="K19" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="13">
         <v>48</v>
       </c>
@@ -1494,17 +1552,17 @@
       <c r="E20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F20" s="72"/>
       <c r="G20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="73"/>
       <c r="I20" s="13"/>
       <c r="K20" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="13">
         <v>49</v>
       </c>
@@ -1520,17 +1578,17 @@
       <c r="E21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="13"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="27"/>
+      <c r="H21" s="73"/>
       <c r="I21" s="13"/>
       <c r="K21" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="51" customFormat="1">
       <c r="A22" s="13">
         <v>50</v>
       </c>
@@ -1542,20 +1600,20 @@
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="72" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="34"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="34"/>
+      <c r="J22" s="33"/>
       <c r="K22" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="51" customFormat="1">
       <c r="A23" s="13">
         <v>51</v>
       </c>
@@ -1565,18 +1623,20 @@
       <c r="C23" s="12">
         <v>45284</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="72"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="55" t="s">
+      <c r="H23" s="52" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="13"/>
-      <c r="J23" s="34"/>
+      <c r="J23" s="33"/>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="9">
         <v>52</v>
       </c>
@@ -1586,18 +1646,18 @@
       <c r="C24" s="12">
         <v>45291</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="67"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
       <c r="K24" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="9">
         <v>1</v>
       </c>
@@ -1607,20 +1667,20 @@
       <c r="C25" s="12">
         <v>45298</v>
       </c>
-      <c r="D25" s="73" t="s">
+      <c r="D25" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="73"/>
       <c r="K25" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="9">
         <v>2</v>
       </c>
@@ -1633,36 +1693,36 @@
       <c r="D26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="13"/>
+      <c r="E26" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="72"/>
       <c r="G26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="27"/>
+      <c r="H26" s="73"/>
       <c r="K26" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+    <row r="27" spans="1:11">
+      <c r="A27" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="20"/>
-      <c r="K27" s="47">
+      <c r="K27" s="45">
         <f>SUM(K5:K26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.6" thickBot="1">
       <c r="A28" s="9">
         <v>3</v>
       </c>
@@ -1678,16 +1738,16 @@
       <c r="E28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="27"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="73"/>
       <c r="K28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="15">
         <v>4</v>
       </c>
@@ -1703,17 +1763,17 @@
       <c r="E29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="13"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="37"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="36"/>
       <c r="K29" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="17">
         <v>5</v>
       </c>
@@ -1729,17 +1789,17 @@
       <c r="E30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="13"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="27"/>
-      <c r="I30" s="37"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="36"/>
       <c r="K30" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="17">
         <v>6</v>
       </c>
@@ -1752,20 +1812,20 @@
       <c r="D31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="13"/>
+      <c r="E31" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="72"/>
       <c r="G31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="27"/>
-      <c r="I31" s="37"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="36"/>
       <c r="K31" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="17">
         <v>7</v>
       </c>
@@ -1775,23 +1835,23 @@
       <c r="C32" s="12">
         <v>45340</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>16</v>
+      <c r="D32" s="82" t="s">
+        <v>29</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="13"/>
+      <c r="F32" s="72"/>
       <c r="G32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="27"/>
-      <c r="I32" s="37"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="36"/>
       <c r="K32" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="18">
         <v>8</v>
       </c>
@@ -1801,18 +1861,18 @@
       <c r="C33" s="19">
         <v>45347</v>
       </c>
-      <c r="D33" s="69" t="s">
+      <c r="D33" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
       <c r="K33" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="17">
         <v>9</v>
       </c>
@@ -1828,17 +1888,17 @@
       <c r="E34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="13"/>
+      <c r="F34" s="72"/>
       <c r="G34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="27"/>
+      <c r="H34" s="73"/>
       <c r="I34" s="13"/>
       <c r="K34" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15.6" thickBot="1">
       <c r="A35" s="21">
         <v>10</v>
       </c>
@@ -1854,49 +1914,49 @@
       <c r="E35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="13"/>
+      <c r="F35" s="72"/>
       <c r="G35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="27"/>
-      <c r="I35" s="38"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="37"/>
       <c r="K35" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="23">
         <v>11</v>
       </c>
-      <c r="B36" s="39">
+      <c r="B36" s="38">
         <v>45362</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C36" s="39">
         <v>45368</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="13"/>
+      <c r="E36" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="72"/>
       <c r="G36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="27"/>
+      <c r="H36" s="73"/>
       <c r="K36" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="9">
         <v>12</v>
       </c>
       <c r="B37" s="12">
         <v>45369</v>
       </c>
-      <c r="C37" s="41">
+      <c r="C37" s="40">
         <v>45375</v>
       </c>
       <c r="D37" s="13" t="s">
@@ -1905,46 +1965,46 @@
       <c r="E37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="13"/>
+      <c r="F37" s="72"/>
       <c r="G37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="27"/>
-      <c r="I37" s="38"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="37"/>
       <c r="K37" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="9">
         <v>13</v>
       </c>
       <c r="B38" s="12">
         <v>45376</v>
       </c>
-      <c r="C38" s="41">
+      <c r="C38" s="40">
         <v>45382</v>
       </c>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="38"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="37"/>
       <c r="K38" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="9">
         <v>14</v>
       </c>
-      <c r="B39" s="42">
+      <c r="B39" s="41">
         <v>45383</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="42">
         <v>45389</v>
       </c>
       <c r="D39" s="24" t="s">
@@ -1953,15 +2013,15 @@
       <c r="E39" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="13"/>
+      <c r="F39" s="72"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="38"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="37"/>
       <c r="K39" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="9">
         <v>15</v>
       </c>
@@ -1977,16 +2037,16 @@
       <c r="E40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="44"/>
+      <c r="F40" s="76"/>
       <c r="G40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="29"/>
+      <c r="H40" s="77"/>
       <c r="K40" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="9">
         <v>16</v>
       </c>
@@ -2002,16 +2062,16 @@
       <c r="E41" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="27"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="73"/>
       <c r="K41" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="9">
         <v>17</v>
       </c>
@@ -2027,16 +2087,16 @@
       <c r="E42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="13"/>
+      <c r="F42" s="72"/>
       <c r="G42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="27"/>
+      <c r="H42" s="73"/>
       <c r="K42" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="9">
         <v>18</v>
       </c>
@@ -2046,24 +2106,24 @@
       <c r="C43" s="12">
         <v>45417</v>
       </c>
-      <c r="D43" s="49" t="s">
+      <c r="D43" s="47" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="48">
+      <c r="F43" s="46">
         <v>45047</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="27"/>
+      <c r="H43" s="73"/>
       <c r="K43" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="9">
         <v>19</v>
       </c>
@@ -2073,24 +2133,24 @@
       <c r="C44" s="12">
         <v>45424</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>16</v>
+      <c r="D44" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="13"/>
+      <c r="F44" s="72"/>
       <c r="G44" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H44" s="46" t="s">
+      <c r="H44" s="44" t="s">
         <v>24</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="9">
         <v>20</v>
       </c>
@@ -2106,19 +2166,19 @@
       <c r="E45" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="49"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="56">
+      <c r="H45" s="53">
         <v>45063</v>
       </c>
-      <c r="I45" s="38"/>
+      <c r="I45" s="37"/>
       <c r="K45" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="9">
         <v>21</v>
       </c>
@@ -2134,18 +2194,18 @@
       <c r="E46" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="52" t="s">
+      <c r="F46" s="72"/>
+      <c r="G46" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="79" t="s">
         <v>16</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="8" customFormat="1">
       <c r="A47" s="9">
         <v>22</v>
       </c>
@@ -2161,18 +2221,18 @@
       <c r="E47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="13"/>
+      <c r="F47" s="72"/>
       <c r="G47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="30"/>
-      <c r="I47" s="38"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="37"/>
       <c r="J47" s="25"/>
       <c r="K47" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="9">
         <v>23</v>
       </c>
@@ -2182,20 +2242,20 @@
       <c r="C48" s="12">
         <v>45452</v>
       </c>
-      <c r="D48" s="51"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="13"/>
+      <c r="F48" s="72"/>
       <c r="G48" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="30"/>
+      <c r="H48" s="80"/>
       <c r="K48" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19">
       <c r="A49" s="9">
         <v>24</v>
       </c>
@@ -2211,17 +2271,17 @@
       <c r="E49" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="13"/>
+      <c r="F49" s="72"/>
       <c r="G49" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="30"/>
-      <c r="I49" s="38"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="37"/>
       <c r="K49" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" s="9">
         <v>25</v>
       </c>
@@ -2237,16 +2297,16 @@
       <c r="E50" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="50" t="s">
+      <c r="F50" s="72"/>
+      <c r="G50" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="H50" s="30"/>
+      <c r="H50" s="29"/>
       <c r="K50" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
       <c r="D51" s="13"/>
@@ -2255,7 +2315,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="27"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="27"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
@@ -2266,38 +2326,38 @@
       <c r="F52" s="28"/>
       <c r="G52" s="28"/>
       <c r="H52" s="27"/>
-      <c r="K52" s="47">
+      <c r="K52" s="45">
         <f>SUM(K28:K51)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
+    <row r="53" spans="1:19">
+      <c r="A53" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="59"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="56"/>
       <c r="I53" s="20"/>
-      <c r="K53" s="47">
+      <c r="K53" s="45">
         <f>K27+K52</f>
         <v>0</v>
       </c>
-      <c r="L53" s="53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I56" s="45"/>
+      <c r="L53" s="50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="I56" s="43"/>
       <c r="K56" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="17.399999999999999">
       <c r="M60" s="3" t="s">
         <v>16</v>
       </c>
@@ -2306,20 +2366,20 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="61" spans="1:19" ht="68.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="68.55" customHeight="1">
       <c r="J61" s="28"/>
       <c r="K61" s="14"/>
-      <c r="L61" s="32"/>
+      <c r="L61" s="31"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="18">
       <c r="J62" s="28"/>
       <c r="K62" s="14"/>
-      <c r="L62" s="32"/>
+      <c r="L62" s="31"/>
       <c r="M62" s="6"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -2327,10 +2387,10 @@
       <c r="Q62" s="6"/>
       <c r="S62" s="2"/>
     </row>
-    <row r="63" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="18">
       <c r="J63" s="28"/>
       <c r="K63" s="14"/>
-      <c r="L63" s="32"/>
+      <c r="L63" s="31"/>
       <c r="M63" s="6"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -2338,10 +2398,10 @@
       <c r="Q63" s="6"/>
       <c r="S63" s="2"/>
     </row>
-    <row r="64" spans="1:19" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J64" s="31"/>
+    <row r="64" spans="1:19" ht="99.6" customHeight="1">
+      <c r="J64" s="30"/>
       <c r="K64" s="12"/>
-      <c r="L64" s="33"/>
+      <c r="L64" s="32"/>
       <c r="M64" s="6"/>
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
@@ -2349,8 +2409,8 @@
       <c r="Q64" s="6"/>
       <c r="S64" s="2"/>
     </row>
-    <row r="65" ht="99.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048575" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" ht="99.6" customHeight="1"/>
+    <row r="1048575" spans="4:4">
       <c r="D1048575" s="13"/>
     </row>
   </sheetData>
@@ -2378,7 +2438,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2392,7 +2452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2410,6 +2470,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003133478D57CB5A4BB798E31C0495E537" ma:contentTypeVersion="5" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="4cdabf6939d7595fe65c5a9933a1a39d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbde4e59-9b61-48a0-a4d9-cce2922754f5" xmlns:ns3="549b603a-3c19-46c1-8987-e792084663ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83240ea6ee18443d145d46ddbabbcefc" ns2:_="" ns3:_="">
     <xsd:import namespace="dbde4e59-9b61-48a0-a4d9-cce2922754f5"/>
@@ -2580,12 +2646,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E35A054-E1C7-4BEB-A605-3B5F23CC3CE4}">
   <ds:schemaRefs>
@@ -2595,6 +2655,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272690DD-D909-48C2-8616-DAB6B7741CC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2611,13 +2680,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
la til oppgave 1.41 - 1.44
</commit_message>
<xml_diff>
--- a/Årsplan IT2.xlsx
+++ b/Årsplan IT2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iktagder-my.sharepoint.com/personal/fredrik_pettersen_mandal_vgs_no/Documents/2023 - 2024/IT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E593647-C825-4342-B68D-65F0866BA014}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308F3CB5-193E-4CEB-A526-112DEEDC6DE2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
   <si>
     <t>Arbeidsplan Naturfag 1IDA</t>
   </si>
@@ -133,6 +133,69 @@
   </si>
   <si>
     <t>Fagdag Blokk 4</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Selvstudie: Strengmetoder</t>
+  </si>
+  <si>
+    <t>Timejustering</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>HTML, CSS, Variabler</t>
+  </si>
+  <si>
+    <t>Variabler med tall</t>
+  </si>
+  <si>
+    <t>Array-metoder, sortering og for-løkker</t>
+  </si>
+  <si>
+    <t>Funksjoner</t>
+  </si>
+  <si>
+    <t>Funksjoner med parametere og returverdier</t>
+  </si>
+  <si>
+    <t>Valgsetninger og flytdiagrammer</t>
+  </si>
+  <si>
+    <t>if-else if-else</t>
+  </si>
+  <si>
+    <t>Logiske operatorer</t>
+  </si>
+  <si>
+    <t>Objekter</t>
+  </si>
+  <si>
+    <t>Oppgave</t>
+  </si>
+  <si>
+    <t>Export og import</t>
+  </si>
+  <si>
+    <t>Komponenter</t>
+  </si>
+  <si>
+    <t>Komponent-egenskaper</t>
+  </si>
+  <si>
+    <t>Lage komponenter</t>
+  </si>
+  <si>
+    <t>Repetisjon</t>
+  </si>
+  <si>
+    <t>Eksamen</t>
+  </si>
+  <si>
+    <t>Eksamen, norsk sidemål</t>
   </si>
 </sst>
 </file>
@@ -142,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ mmm\."/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,7 +268,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +323,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -512,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -669,6 +744,39 @@
     <xf numFmtId="16" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,38 +831,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -778,6 +859,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,11 +1158,11 @@
   <dimension ref="A1:S1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.21875" style="25" customWidth="1"/>
     <col min="2" max="3" width="9.5546875" style="25" customWidth="1"/>
@@ -1096,31 +1181,31 @@
     <col min="17" max="18" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="59"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1135,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1161,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>33</v>
       </c>
@@ -1171,18 +1256,18 @@
       <c r="C5" s="12">
         <v>45158</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="73"/>
+      <c r="H5" s="55"/>
       <c r="K5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>34</v>
       </c>
@@ -1193,22 +1278,22 @@
         <v>45165</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="72"/>
+        <v>37</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="73"/>
+        <v>38</v>
+      </c>
+      <c r="H6" s="55"/>
       <c r="I6" s="13"/>
-      <c r="K6" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="K6" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>35</v>
       </c>
@@ -1219,22 +1304,22 @@
         <v>45172</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="72"/>
+        <v>34</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="73"/>
+        <v>33</v>
+      </c>
+      <c r="H7" s="55"/>
       <c r="I7" s="13"/>
-      <c r="K7" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>36</v>
       </c>
@@ -1245,21 +1330,21 @@
         <v>45179</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="72"/>
+        <v>40</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="73"/>
-      <c r="K8" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>41</v>
+      </c>
+      <c r="H8" s="55"/>
+      <c r="K8" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>37</v>
       </c>
@@ -1270,21 +1355,21 @@
         <v>45186</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="72"/>
+        <v>43</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="73"/>
-      <c r="K9" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1">
+        <v>44</v>
+      </c>
+      <c r="H9" s="55"/>
+      <c r="K9" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>38</v>
       </c>
@@ -1295,23 +1380,23 @@
         <v>45193</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="73"/>
+        <v>45</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="55"/>
       <c r="I10" s="9"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="K10" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>39</v>
       </c>
@@ -1322,21 +1407,21 @@
         <v>45200</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="72"/>
+        <v>48</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="73"/>
-      <c r="K11" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>48</v>
+      </c>
+      <c r="H11" s="55"/>
+      <c r="K11" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>40</v>
       </c>
@@ -1346,18 +1431,18 @@
       <c r="C12" s="14">
         <v>45207</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
       <c r="K12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>41</v>
       </c>
@@ -1368,22 +1453,22 @@
         <v>45214</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="72"/>
+        <v>49</v>
+      </c>
+      <c r="F13" s="54"/>
       <c r="G13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="74"/>
+        <v>50</v>
+      </c>
+      <c r="H13" s="56"/>
       <c r="I13" s="13"/>
-      <c r="K13" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="K13" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>42</v>
       </c>
@@ -1394,23 +1479,23 @@
         <v>45221</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="54"/>
+      <c r="G14" s="63" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K14" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>43</v>
       </c>
@@ -1426,17 +1511,17 @@
       <c r="E15" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="72"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="73"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="13"/>
-      <c r="K15" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="K15" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>44</v>
       </c>
@@ -1452,16 +1537,16 @@
       <c r="E16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="72"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="73"/>
-      <c r="K16" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="H16" s="55"/>
+      <c r="K16" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>45</v>
       </c>
@@ -1477,16 +1562,16 @@
       <c r="E17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="72"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="73"/>
-      <c r="K17" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="H17" s="55"/>
+      <c r="K17" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>46</v>
       </c>
@@ -1502,16 +1587,16 @@
       <c r="E18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="72"/>
+      <c r="F18" s="54"/>
       <c r="G18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="K18" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="H18" s="55"/>
+      <c r="K18" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>47</v>
       </c>
@@ -1524,19 +1609,19 @@
       <c r="D19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="81" t="s">
+      <c r="E19" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="72"/>
+      <c r="F19" s="54"/>
       <c r="G19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="K19" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="H19" s="55"/>
+      <c r="K19" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>48</v>
       </c>
@@ -1552,17 +1637,17 @@
       <c r="E20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="72"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="73"/>
+      <c r="H20" s="55"/>
       <c r="I20" s="13"/>
-      <c r="K20" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="K20" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>49</v>
       </c>
@@ -1578,17 +1663,17 @@
       <c r="E21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="72"/>
+      <c r="F21" s="54"/>
       <c r="G21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="73"/>
+      <c r="H21" s="55"/>
       <c r="I21" s="13"/>
-      <c r="K21" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="51" customFormat="1">
+      <c r="K21" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>50</v>
       </c>
@@ -1600,20 +1685,20 @@
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="54" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="57"/>
       <c r="I22" s="13"/>
       <c r="J22" s="33"/>
-      <c r="K22" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="51" customFormat="1">
+      <c r="K22" s="13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>51</v>
       </c>
@@ -1627,16 +1712,18 @@
         <v>31</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="72"/>
+      <c r="F23" s="54"/>
       <c r="G23" s="13"/>
       <c r="H23" s="52" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="33"/>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="K23" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>52</v>
       </c>
@@ -1646,18 +1733,18 @@
       <c r="C24" s="12">
         <v>45291</v>
       </c>
-      <c r="D24" s="64" t="s">
+      <c r="D24" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="64"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
       <c r="K24" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>1</v>
       </c>
@@ -1667,20 +1754,20 @@
       <c r="C25" s="12">
         <v>45298</v>
       </c>
-      <c r="D25" s="70" t="s">
+      <c r="D25" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="71"/>
-      <c r="F25" s="72"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="73"/>
-      <c r="K25" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="H25" s="55"/>
+      <c r="K25" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>2</v>
       </c>
@@ -1693,36 +1780,36 @@
       <c r="D26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="81" t="s">
+      <c r="E26" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="72"/>
+      <c r="F26" s="54"/>
       <c r="G26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="73"/>
-      <c r="K26" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="54" t="s">
+      <c r="H26" s="55"/>
+      <c r="K26" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
       <c r="I27" s="20"/>
       <c r="K27" s="45">
         <f>SUM(K5:K26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.6" thickBot="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>3</v>
       </c>
@@ -1738,16 +1825,16 @@
       <c r="E28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="72"/>
+      <c r="F28" s="54"/>
       <c r="G28" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="73"/>
-      <c r="K28" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="H28" s="55"/>
+      <c r="K28" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>4</v>
       </c>
@@ -1763,17 +1850,17 @@
       <c r="E29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="72"/>
+      <c r="F29" s="54"/>
       <c r="G29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="73"/>
+      <c r="H29" s="55"/>
       <c r="I29" s="36"/>
-      <c r="K29" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="K29" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>5</v>
       </c>
@@ -1789,17 +1876,17 @@
       <c r="E30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="72"/>
+      <c r="F30" s="54"/>
       <c r="G30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="73"/>
+      <c r="H30" s="55"/>
       <c r="I30" s="36"/>
-      <c r="K30" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="K30" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>6</v>
       </c>
@@ -1812,20 +1899,20 @@
       <c r="D31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="81" t="s">
+      <c r="E31" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="72"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="73"/>
+      <c r="H31" s="55"/>
       <c r="I31" s="36"/>
-      <c r="K31" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="K31" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>7</v>
       </c>
@@ -1835,23 +1922,23 @@
       <c r="C32" s="12">
         <v>45340</v>
       </c>
-      <c r="D32" s="82" t="s">
+      <c r="D32" s="64" t="s">
         <v>29</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="72"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="73"/>
+      <c r="H32" s="55"/>
       <c r="I32" s="36"/>
-      <c r="K32" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="K32" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>8</v>
       </c>
@@ -1861,18 +1948,18 @@
       <c r="C33" s="19">
         <v>45347</v>
       </c>
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
       <c r="K33" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>9</v>
       </c>
@@ -1888,17 +1975,17 @@
       <c r="E34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="72"/>
+      <c r="F34" s="54"/>
       <c r="G34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="73"/>
+      <c r="H34" s="55"/>
       <c r="I34" s="13"/>
-      <c r="K34" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.6" thickBot="1">
+      <c r="K34" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
         <v>10</v>
       </c>
@@ -1914,17 +2001,17 @@
       <c r="E35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="72"/>
+      <c r="F35" s="54"/>
       <c r="G35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="73"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="37"/>
-      <c r="K35" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="K35" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>11</v>
       </c>
@@ -1937,19 +2024,19 @@
       <c r="D36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="81" t="s">
+      <c r="E36" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="72"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="73"/>
-      <c r="K36" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="H36" s="55"/>
+      <c r="K36" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>12</v>
       </c>
@@ -1965,17 +2052,17 @@
       <c r="E37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="72"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="73"/>
+      <c r="H37" s="55"/>
       <c r="I37" s="37"/>
-      <c r="K37" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="K37" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>13</v>
       </c>
@@ -1985,19 +2072,19 @@
       <c r="C38" s="40">
         <v>45382</v>
       </c>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="69"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="80"/>
       <c r="I38" s="37"/>
       <c r="K38" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>14</v>
       </c>
@@ -2013,15 +2100,15 @@
       <c r="E39" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="72"/>
+      <c r="F39" s="54"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="73"/>
+      <c r="H39" s="55"/>
       <c r="I39" s="37"/>
-      <c r="K39" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="K39" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>15</v>
       </c>
@@ -2037,16 +2124,16 @@
       <c r="E40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="76"/>
+      <c r="F40" s="58"/>
       <c r="G40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="77"/>
-      <c r="K40" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="H40" s="59"/>
+      <c r="K40" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>16</v>
       </c>
@@ -2062,16 +2149,16 @@
       <c r="E41" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="72"/>
-      <c r="G41" s="81" t="s">
+      <c r="F41" s="54"/>
+      <c r="G41" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="73"/>
-      <c r="K41" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="H41" s="55"/>
+      <c r="K41" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>17</v>
       </c>
@@ -2087,16 +2174,16 @@
       <c r="E42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="72"/>
+      <c r="F42" s="54"/>
       <c r="G42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="73"/>
-      <c r="K42" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="H42" s="55"/>
+      <c r="K42" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>18</v>
       </c>
@@ -2118,12 +2205,12 @@
       <c r="G43" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="73"/>
-      <c r="K43" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="H43" s="55"/>
+      <c r="K43" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>19</v>
       </c>
@@ -2139,18 +2226,18 @@
       <c r="E44" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="72"/>
+      <c r="F44" s="54"/>
       <c r="G44" s="24" t="s">
         <v>23</v>
       </c>
       <c r="H44" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K44" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="K44" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>20</v>
       </c>
@@ -2166,7 +2253,7 @@
       <c r="E45" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="78"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="13" t="s">
         <v>16</v>
       </c>
@@ -2174,11 +2261,11 @@
         <v>45063</v>
       </c>
       <c r="I45" s="37"/>
-      <c r="K45" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="K45" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>21</v>
       </c>
@@ -2191,21 +2278,21 @@
       <c r="D46" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="72"/>
+      <c r="E46" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="54"/>
       <c r="G46" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="8" customFormat="1">
+      <c r="H46" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>22</v>
       </c>
@@ -2221,18 +2308,18 @@
       <c r="E47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="72"/>
-      <c r="G47" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="80"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="62"/>
       <c r="I47" s="37"/>
       <c r="J47" s="25"/>
-      <c r="K47" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="K47" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>23</v>
       </c>
@@ -2246,16 +2333,16 @@
       <c r="E48" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="72"/>
+      <c r="F48" s="54"/>
       <c r="G48" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="80"/>
-      <c r="K48" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="H48" s="62"/>
+      <c r="K48" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>24</v>
       </c>
@@ -2271,17 +2358,17 @@
       <c r="E49" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="72"/>
+      <c r="F49" s="54"/>
       <c r="G49" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="80"/>
+      <c r="H49" s="62"/>
       <c r="I49" s="37"/>
-      <c r="K49" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="K49" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>25</v>
       </c>
@@ -2291,22 +2378,19 @@
       <c r="C50" s="12">
         <v>45466</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="72"/>
+      <c r="D50" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="54"/>
       <c r="G50" s="48" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="29"/>
-      <c r="K50" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19">
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
       <c r="D51" s="13"/>
@@ -2315,7 +2399,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="27"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
@@ -2328,36 +2412,36 @@
       <c r="H52" s="27"/>
       <c r="K52" s="45">
         <f>SUM(K28:K51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" s="54" t="s">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="56"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="67"/>
       <c r="I53" s="20"/>
       <c r="K53" s="45">
         <f>K27+K52</f>
-        <v>0</v>
+        <v>159.5</v>
       </c>
       <c r="L53" s="50" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I56" s="43"/>
       <c r="K56" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="17.399999999999999">
+    <row r="60" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="M60" s="3" t="s">
         <v>16</v>
       </c>
@@ -2366,7 +2450,7 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="61" spans="1:19" ht="68.55" customHeight="1">
+    <row r="61" spans="1:19" ht="68.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J61" s="28"/>
       <c r="K61" s="14"/>
       <c r="L61" s="31"/>
@@ -2376,7 +2460,7 @@
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:19" ht="18">
+    <row r="62" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="J62" s="28"/>
       <c r="K62" s="14"/>
       <c r="L62" s="31"/>
@@ -2387,7 +2471,7 @@
       <c r="Q62" s="6"/>
       <c r="S62" s="2"/>
     </row>
-    <row r="63" spans="1:19" ht="18">
+    <row r="63" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="J63" s="28"/>
       <c r="K63" s="14"/>
       <c r="L63" s="31"/>
@@ -2398,7 +2482,7 @@
       <c r="Q63" s="6"/>
       <c r="S63" s="2"/>
     </row>
-    <row r="64" spans="1:19" ht="99.6" customHeight="1">
+    <row r="64" spans="1:19" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J64" s="30"/>
       <c r="K64" s="12"/>
       <c r="L64" s="32"/>
@@ -2409,8 +2493,8 @@
       <c r="Q64" s="6"/>
       <c r="S64" s="2"/>
     </row>
-    <row r="65" ht="99.6" customHeight="1"/>
-    <row r="1048575" spans="4:4">
+    <row r="65" ht="99.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048575" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D1048575" s="13"/>
     </row>
   </sheetData>
@@ -2438,7 +2522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2452,7 +2536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -2470,12 +2554,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003133478D57CB5A4BB798E31C0495E537" ma:contentTypeVersion="5" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="4cdabf6939d7595fe65c5a9933a1a39d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbde4e59-9b61-48a0-a4d9-cce2922754f5" xmlns:ns3="549b603a-3c19-46c1-8987-e792084663ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83240ea6ee18443d145d46ddbabbcefc" ns2:_="" ns3:_="">
     <xsd:import namespace="dbde4e59-9b61-48a0-a4d9-cce2922754f5"/>
@@ -2646,6 +2724,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E35A054-E1C7-4BEB-A605-3B5F23CC3CE4}">
   <ds:schemaRefs>
@@ -2655,15 +2739,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272690DD-D909-48C2-8616-DAB6B7741CC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2680,4 +2755,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ferdig delkapittel 1.6 og lagt til noen fra delkapittel 1.1
</commit_message>
<xml_diff>
--- a/Årsplan IT2.xlsx
+++ b/Årsplan IT2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iktagder-my.sharepoint.com/personal/fredrik_pettersen_mandal_vgs_no/Documents/2023 - 2024/IT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308F3CB5-193E-4CEB-A526-112DEEDC6DE2}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{865BB95E-C4AD-467E-BA78-E08323D10E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5612BF-CF5A-4769-9B8E-E479C0AE5421}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
   <si>
     <t>Arbeidsplan Naturfag 1IDA</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Objekter</t>
-  </si>
-  <si>
-    <t>Oppgave</t>
   </si>
   <si>
     <t>Export og import</t>
@@ -268,7 +265,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,12 +322,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -777,6 +768,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,10 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1158,8 +1149,8 @@
   <dimension ref="A1:S1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+      <pane ySplit="4" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,28 +1173,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
@@ -1382,12 +1373,12 @@
       <c r="D10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="84" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="83" t="s">
-        <v>46</v>
       </c>
       <c r="H10" s="55"/>
       <c r="I10" s="9"/>
@@ -1407,14 +1398,14 @@
         <v>45200</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="F11" s="54"/>
       <c r="G11" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="55"/>
       <c r="K11" s="9">
@@ -1431,13 +1422,13 @@
       <c r="C12" s="14">
         <v>45207</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
       <c r="K12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1453,14 +1444,14 @@
         <v>45214</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="54"/>
       <c r="G13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" s="56"/>
       <c r="I13" s="13"/>
@@ -1479,10 +1470,10 @@
         <v>45221</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="63" t="s">
@@ -1733,13 +1724,13 @@
       <c r="C24" s="12">
         <v>45291</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
       <c r="K24" s="9" t="s">
         <v>16</v>
       </c>
@@ -1754,10 +1745,10 @@
       <c r="C25" s="12">
         <v>45298</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="82"/>
+      <c r="E25" s="83"/>
       <c r="F25" s="54"/>
       <c r="G25" s="13" t="s">
         <v>16</v>
@@ -1793,16 +1784,16 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="68"/>
       <c r="I27" s="20"/>
       <c r="K27" s="45">
         <f>SUM(K5:K26)</f>
@@ -1948,13 +1939,13 @@
       <c r="C33" s="19">
         <v>45347</v>
       </c>
-      <c r="D33" s="77" t="s">
+      <c r="D33" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
       <c r="K33" s="9" t="s">
         <v>16</v>
       </c>
@@ -2072,13 +2063,13 @@
       <c r="C38" s="40">
         <v>45382</v>
       </c>
-      <c r="D38" s="78" t="s">
+      <c r="D38" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="81"/>
       <c r="I38" s="37"/>
       <c r="K38" s="9" t="s">
         <v>16</v>
@@ -2279,7 +2270,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F46" s="54"/>
       <c r="G46" s="47" t="s">
@@ -2309,8 +2300,8 @@
         <v>16</v>
       </c>
       <c r="F47" s="54"/>
-      <c r="G47" s="84" t="s">
-        <v>52</v>
+      <c r="G47" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="H47" s="62"/>
       <c r="I47" s="37"/>
@@ -2416,16 +2407,16 @@
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="s">
+      <c r="A53" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="66"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="66"/>
-      <c r="F53" s="66"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="67"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="68"/>
       <c r="I53" s="20"/>
       <c r="K53" s="45">
         <f>K27+K52</f>
@@ -2554,6 +2545,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003133478D57CB5A4BB798E31C0495E537" ma:contentTypeVersion="5" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="4cdabf6939d7595fe65c5a9933a1a39d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbde4e59-9b61-48a0-a4d9-cce2922754f5" xmlns:ns3="549b603a-3c19-46c1-8987-e792084663ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83240ea6ee18443d145d46ddbabbcefc" ns2:_="" ns3:_="">
     <xsd:import namespace="dbde4e59-9b61-48a0-a4d9-cce2922754f5"/>
@@ -2724,12 +2721,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E35A054-E1C7-4BEB-A605-3B5F23CC3CE4}">
   <ds:schemaRefs>
@@ -2739,6 +2730,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272690DD-D909-48C2-8616-DAB6B7741CC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2755,13 +2755,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B07430-6BCC-4282-8F52-297D885FAD4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>